<commit_message>
carga de imagen al reporte
</commit_message>
<xml_diff>
--- a/test/reporte_inscripciones_evento_1.xlsx
+++ b/test/reporte_inscripciones_evento_1.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,6 +511,168 @@
       <c r="E4" t="inlineStr">
         <is>
           <t>qllo</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Claure Reyes</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Milenia</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Centro Cultural Anglo Americano Cochabamba</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Cochabamba</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Cercado</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Argote Gomez</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Noelia</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Colegio Particular Hispano Boliviano</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Cochabamba</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Cercado</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Azogue Aranibar</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Fernando</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Colegio Particular Hispano Boliviano</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Cochabamba</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Cercado</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Galvez Perez</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Rodrigo</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Centro Cultural Anglo Americano Cochabamba</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Cochabamba</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Sacaba</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Gonzales Medrano</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Emilio Jorge</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Colegio Loyola</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Cochabamba</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Cercado</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Vega Salinas</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Juan Pablo</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Colegio Albert Einstein</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Cochabamba</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Cercado</t>
         </is>
       </c>
     </row>

</xml_diff>